<commit_message>
complete create final_stop_times section
- edit timetable_output_table.xlsx in Excel
- create final_stop_times
</commit_message>
<xml_diff>
--- a/data/timetable_output_table.xlsx
+++ b/data/timetable_output_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\herşey\R_projects\GTFS_for_Athens\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C6694A-E9A3-4A3C-94C4-C7ED041A25AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40490185-8E69-451A-A402-9FD8CAE07C7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -799,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C238" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I237" sqref="I237"/>
+    <sheetView tabSelected="1" topLeftCell="A217" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C250" sqref="C250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7000,7 +7000,7 @@
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A243">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B243" t="s">
         <v>110</v>
@@ -7024,7 +7024,7 @@
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A244">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B244" t="s">
         <v>110</v>
@@ -7048,7 +7048,7 @@
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A245">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B245" t="s">
         <v>110</v>

</xml_diff>

<commit_message>
fix trip_id's of stop times table
- and create validation.rmd
</commit_message>
<xml_diff>
--- a/data/timetable_output_table.xlsx
+++ b/data/timetable_output_table.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\herşey\R_projects\GTFS_for_Athens\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40490185-8E69-451A-A402-9FD8CAE07C7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C6ED5E-7500-4CCC-927B-9A2D6237FB73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$I$245</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="149">
   <si>
     <t>route_id</t>
   </si>
@@ -456,6 +459,27 @@
   </si>
   <si>
     <t>94 Columbus Rd</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>L6</t>
+  </si>
+  <si>
+    <t>L7n</t>
+  </si>
+  <si>
+    <t>L7a</t>
   </si>
 </sst>
 </file>
@@ -799,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C250" sqref="C250"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -841,8 +865,8 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>53</v>
+      <c r="A2" t="s">
+        <v>142</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -868,8 +892,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>53</v>
+      <c r="A3" t="s">
+        <v>142</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -892,8 +916,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>53</v>
+      <c r="A4" t="s">
+        <v>142</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -916,8 +940,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>53</v>
+      <c r="A5" t="s">
+        <v>142</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -940,8 +964,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>53</v>
+      <c r="A6" t="s">
+        <v>142</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -964,8 +988,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>53</v>
+      <c r="A7" t="s">
+        <v>142</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -988,8 +1012,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>53</v>
+      <c r="A8" t="s">
+        <v>142</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -1012,8 +1036,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>53</v>
+      <c r="A9" t="s">
+        <v>142</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -1036,8 +1060,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>53</v>
+      <c r="A10" t="s">
+        <v>142</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -1060,8 +1084,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>53</v>
+      <c r="A11" t="s">
+        <v>142</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -1084,8 +1108,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>53</v>
+      <c r="A12" t="s">
+        <v>142</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -1108,8 +1132,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>53</v>
+      <c r="A13" t="s">
+        <v>142</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
@@ -1132,8 +1156,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>53</v>
+      <c r="A14" t="s">
+        <v>142</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -1156,8 +1180,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>53</v>
+      <c r="A15" t="s">
+        <v>142</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
@@ -1180,8 +1204,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>53</v>
+      <c r="A16" t="s">
+        <v>142</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
@@ -1204,8 +1228,8 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>53</v>
+      <c r="A17" t="s">
+        <v>142</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
@@ -1228,8 +1252,8 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>53</v>
+      <c r="A18" t="s">
+        <v>142</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
@@ -1252,8 +1276,8 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>53</v>
+      <c r="A19" t="s">
+        <v>142</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
@@ -1276,8 +1300,8 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>53</v>
+      <c r="A20" t="s">
+        <v>142</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
@@ -1303,8 +1327,8 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>53</v>
+      <c r="A21" t="s">
+        <v>142</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
@@ -1327,8 +1351,8 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>53</v>
+      <c r="A22" t="s">
+        <v>142</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
@@ -1351,8 +1375,8 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>53</v>
+      <c r="A23" t="s">
+        <v>142</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -1375,8 +1399,8 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>53</v>
+      <c r="A24" t="s">
+        <v>142</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
@@ -1399,8 +1423,8 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>53</v>
+      <c r="A25" t="s">
+        <v>142</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
@@ -1423,8 +1447,8 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>53</v>
+      <c r="A26" t="s">
+        <v>142</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -1447,8 +1471,8 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <v>53</v>
+      <c r="A27" t="s">
+        <v>142</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
@@ -1471,8 +1495,8 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>53</v>
+      <c r="A28" t="s">
+        <v>142</v>
       </c>
       <c r="B28" t="s">
         <v>5</v>
@@ -1495,8 +1519,8 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29">
-        <v>53</v>
+      <c r="A29" t="s">
+        <v>142</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
@@ -1519,8 +1543,8 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30">
-        <v>53</v>
+      <c r="A30" t="s">
+        <v>142</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
@@ -1543,8 +1567,8 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31">
-        <v>53</v>
+      <c r="A31" t="s">
+        <v>142</v>
       </c>
       <c r="B31" t="s">
         <v>5</v>
@@ -1567,8 +1591,8 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32">
-        <v>53</v>
+      <c r="A32" t="s">
+        <v>142</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
@@ -1591,8 +1615,8 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33">
-        <v>53</v>
+      <c r="A33" t="s">
+        <v>142</v>
       </c>
       <c r="B33" t="s">
         <v>5</v>
@@ -1615,8 +1639,8 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34">
-        <v>53</v>
+      <c r="A34" t="s">
+        <v>142</v>
       </c>
       <c r="B34" t="s">
         <v>5</v>
@@ -1639,8 +1663,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35">
-        <v>53</v>
+      <c r="A35" t="s">
+        <v>142</v>
       </c>
       <c r="B35" t="s">
         <v>5</v>
@@ -1663,8 +1687,8 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36">
-        <v>53</v>
+      <c r="A36" t="s">
+        <v>142</v>
       </c>
       <c r="B36" t="s">
         <v>5</v>
@@ -1687,8 +1711,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37">
-        <v>53</v>
+      <c r="A37" t="s">
+        <v>142</v>
       </c>
       <c r="B37" t="s">
         <v>5</v>
@@ -1711,8 +1735,8 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38">
-        <v>53</v>
+      <c r="A38" t="s">
+        <v>142</v>
       </c>
       <c r="B38" t="s">
         <v>5</v>
@@ -1735,8 +1759,8 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39">
-        <v>53</v>
+      <c r="A39" t="s">
+        <v>142</v>
       </c>
       <c r="B39" t="s">
         <v>5</v>
@@ -1759,8 +1783,8 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40">
-        <v>53</v>
+      <c r="A40" t="s">
+        <v>142</v>
       </c>
       <c r="B40" t="s">
         <v>5</v>
@@ -1783,8 +1807,8 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41">
-        <v>53</v>
+      <c r="A41" t="s">
+        <v>142</v>
       </c>
       <c r="B41" t="s">
         <v>5</v>
@@ -1807,8 +1831,8 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42">
-        <v>53</v>
+      <c r="A42" t="s">
+        <v>142</v>
       </c>
       <c r="B42" t="s">
         <v>5</v>
@@ -1831,8 +1855,8 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43">
-        <v>53</v>
+      <c r="A43" t="s">
+        <v>142</v>
       </c>
       <c r="B43" t="s">
         <v>5</v>
@@ -1855,8 +1879,8 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A44">
-        <v>53</v>
+      <c r="A44" t="s">
+        <v>142</v>
       </c>
       <c r="B44" t="s">
         <v>5</v>
@@ -1879,8 +1903,8 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A45">
-        <v>53</v>
+      <c r="A45" t="s">
+        <v>142</v>
       </c>
       <c r="B45" t="s">
         <v>5</v>
@@ -1904,8 +1928,8 @@
       <c r="I45" s="2"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A46">
-        <v>54</v>
+      <c r="A46" t="s">
+        <v>143</v>
       </c>
       <c r="B46" t="s">
         <v>46</v>
@@ -1928,8 +1952,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A47">
-        <v>54</v>
+      <c r="A47" t="s">
+        <v>143</v>
       </c>
       <c r="B47" t="s">
         <v>46</v>
@@ -1952,8 +1976,8 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A48">
-        <v>54</v>
+      <c r="A48" t="s">
+        <v>143</v>
       </c>
       <c r="B48" t="s">
         <v>46</v>
@@ -1979,8 +2003,8 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A49">
-        <v>54</v>
+      <c r="A49" t="s">
+        <v>143</v>
       </c>
       <c r="B49" t="s">
         <v>46</v>
@@ -2006,8 +2030,8 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A50">
-        <v>54</v>
+      <c r="A50" t="s">
+        <v>143</v>
       </c>
       <c r="B50" t="s">
         <v>46</v>
@@ -2030,8 +2054,8 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A51">
-        <v>54</v>
+      <c r="A51" t="s">
+        <v>143</v>
       </c>
       <c r="B51" t="s">
         <v>46</v>
@@ -2054,8 +2078,8 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A52">
-        <v>54</v>
+      <c r="A52" t="s">
+        <v>143</v>
       </c>
       <c r="B52" t="s">
         <v>46</v>
@@ -2078,8 +2102,8 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A53">
-        <v>54</v>
+      <c r="A53" t="s">
+        <v>143</v>
       </c>
       <c r="B53" t="s">
         <v>46</v>
@@ -2102,8 +2126,8 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A54">
-        <v>54</v>
+      <c r="A54" t="s">
+        <v>143</v>
       </c>
       <c r="B54" t="s">
         <v>46</v>
@@ -2126,8 +2150,8 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A55">
-        <v>54</v>
+      <c r="A55" t="s">
+        <v>143</v>
       </c>
       <c r="B55" t="s">
         <v>46</v>
@@ -2149,8 +2173,8 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A56">
-        <v>54</v>
+      <c r="A56" t="s">
+        <v>143</v>
       </c>
       <c r="B56" t="s">
         <v>46</v>
@@ -2173,8 +2197,8 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A57">
-        <v>54</v>
+      <c r="A57" t="s">
+        <v>143</v>
       </c>
       <c r="B57" t="s">
         <v>46</v>
@@ -2197,8 +2221,8 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A58">
-        <v>54</v>
+      <c r="A58" t="s">
+        <v>143</v>
       </c>
       <c r="B58" t="s">
         <v>46</v>
@@ -2221,8 +2245,8 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A59">
-        <v>54</v>
+      <c r="A59" t="s">
+        <v>143</v>
       </c>
       <c r="B59" t="s">
         <v>46</v>
@@ -2245,8 +2269,8 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A60">
-        <v>54</v>
+      <c r="A60" t="s">
+        <v>143</v>
       </c>
       <c r="B60" t="s">
         <v>46</v>
@@ -2269,8 +2293,8 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A61">
-        <v>54</v>
+      <c r="A61" t="s">
+        <v>143</v>
       </c>
       <c r="B61" t="s">
         <v>46</v>
@@ -2293,8 +2317,8 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A62">
-        <v>54</v>
+      <c r="A62" t="s">
+        <v>143</v>
       </c>
       <c r="B62" t="s">
         <v>46</v>
@@ -2317,8 +2341,8 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A63">
-        <v>54</v>
+      <c r="A63" t="s">
+        <v>143</v>
       </c>
       <c r="B63" t="s">
         <v>46</v>
@@ -2341,8 +2365,8 @@
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A64">
-        <v>54</v>
+      <c r="A64" t="s">
+        <v>143</v>
       </c>
       <c r="B64" t="s">
         <v>46</v>
@@ -2365,8 +2389,8 @@
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A65">
-        <v>54</v>
+      <c r="A65" t="s">
+        <v>143</v>
       </c>
       <c r="B65" t="s">
         <v>46</v>
@@ -2389,8 +2413,8 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A66">
-        <v>54</v>
+      <c r="A66" t="s">
+        <v>143</v>
       </c>
       <c r="B66" t="s">
         <v>46</v>
@@ -2413,8 +2437,8 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A67">
-        <v>54</v>
+      <c r="A67" t="s">
+        <v>143</v>
       </c>
       <c r="B67" t="s">
         <v>46</v>
@@ -2437,8 +2461,8 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A68">
-        <v>54</v>
+      <c r="A68" t="s">
+        <v>143</v>
       </c>
       <c r="B68" t="s">
         <v>46</v>
@@ -2461,8 +2485,8 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A69">
-        <v>54</v>
+      <c r="A69" t="s">
+        <v>143</v>
       </c>
       <c r="B69" t="s">
         <v>46</v>
@@ -2485,8 +2509,8 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A70">
-        <v>54</v>
+      <c r="A70" t="s">
+        <v>143</v>
       </c>
       <c r="B70" t="s">
         <v>46</v>
@@ -2512,8 +2536,8 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A71">
-        <v>54</v>
+      <c r="A71" t="s">
+        <v>143</v>
       </c>
       <c r="B71" t="s">
         <v>46</v>
@@ -2536,8 +2560,8 @@
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A72">
-        <v>54</v>
+      <c r="A72" t="s">
+        <v>143</v>
       </c>
       <c r="B72" t="s">
         <v>46</v>
@@ -2560,8 +2584,8 @@
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A73">
-        <v>54</v>
+      <c r="A73" t="s">
+        <v>143</v>
       </c>
       <c r="B73" t="s">
         <v>46</v>
@@ -2584,8 +2608,8 @@
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A74">
-        <v>54</v>
+      <c r="A74" t="s">
+        <v>143</v>
       </c>
       <c r="B74" t="s">
         <v>46</v>
@@ -2608,8 +2632,8 @@
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A75">
-        <v>54</v>
+      <c r="A75" t="s">
+        <v>143</v>
       </c>
       <c r="B75" t="s">
         <v>46</v>
@@ -2632,8 +2656,8 @@
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A76">
-        <v>54</v>
+      <c r="A76" t="s">
+        <v>143</v>
       </c>
       <c r="B76" t="s">
         <v>46</v>
@@ -2656,8 +2680,8 @@
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A77">
-        <v>54</v>
+      <c r="A77" t="s">
+        <v>143</v>
       </c>
       <c r="B77" t="s">
         <v>46</v>
@@ -2680,8 +2704,8 @@
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A78">
-        <v>54</v>
+      <c r="A78" t="s">
+        <v>143</v>
       </c>
       <c r="B78" t="s">
         <v>46</v>
@@ -2704,8 +2728,8 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A79">
-        <v>54</v>
+      <c r="A79" t="s">
+        <v>143</v>
       </c>
       <c r="B79" t="s">
         <v>46</v>
@@ -2728,8 +2752,8 @@
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A80">
-        <v>54</v>
+      <c r="A80" t="s">
+        <v>143</v>
       </c>
       <c r="B80" t="s">
         <v>46</v>
@@ -2752,8 +2776,8 @@
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A81">
-        <v>54</v>
+      <c r="A81" t="s">
+        <v>143</v>
       </c>
       <c r="B81" t="s">
         <v>46</v>
@@ -2776,8 +2800,8 @@
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A82">
-        <v>54</v>
+      <c r="A82" t="s">
+        <v>143</v>
       </c>
       <c r="B82" t="s">
         <v>46</v>
@@ -2800,8 +2824,8 @@
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A83">
-        <v>54</v>
+      <c r="A83" t="s">
+        <v>143</v>
       </c>
       <c r="B83" t="s">
         <v>46</v>
@@ -2824,8 +2848,8 @@
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A84">
-        <v>54</v>
+      <c r="A84" t="s">
+        <v>143</v>
       </c>
       <c r="B84" t="s">
         <v>46</v>
@@ -2848,8 +2872,8 @@
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A85">
-        <v>54</v>
+      <c r="A85" t="s">
+        <v>143</v>
       </c>
       <c r="B85" t="s">
         <v>46</v>
@@ -2872,8 +2896,8 @@
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A86">
-        <v>54</v>
+      <c r="A86" t="s">
+        <v>143</v>
       </c>
       <c r="B86" t="s">
         <v>46</v>
@@ -2896,8 +2920,8 @@
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A87">
-        <v>54</v>
+      <c r="A87" t="s">
+        <v>143</v>
       </c>
       <c r="B87" t="s">
         <v>46</v>
@@ -2920,8 +2944,8 @@
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A88">
-        <v>54</v>
+      <c r="A88" t="s">
+        <v>143</v>
       </c>
       <c r="B88" t="s">
         <v>46</v>
@@ -2944,8 +2968,8 @@
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A89">
-        <v>54</v>
+      <c r="A89" t="s">
+        <v>143</v>
       </c>
       <c r="B89" t="s">
         <v>46</v>
@@ -2971,8 +2995,8 @@
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A90">
-        <v>54</v>
+      <c r="A90" t="s">
+        <v>143</v>
       </c>
       <c r="B90" t="s">
         <v>46</v>
@@ -2998,8 +3022,8 @@
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A91">
-        <v>55</v>
+      <c r="A91" t="s">
+        <v>144</v>
       </c>
       <c r="B91" t="s">
         <v>52</v>
@@ -3022,8 +3046,8 @@
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A92">
-        <v>55</v>
+      <c r="A92" t="s">
+        <v>144</v>
       </c>
       <c r="B92" t="s">
         <v>52</v>
@@ -3046,8 +3070,8 @@
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A93">
-        <v>55</v>
+      <c r="A93" t="s">
+        <v>144</v>
       </c>
       <c r="B93" t="s">
         <v>52</v>
@@ -3070,8 +3094,8 @@
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A94">
-        <v>55</v>
+      <c r="A94" t="s">
+        <v>144</v>
       </c>
       <c r="B94" t="s">
         <v>52</v>
@@ -3094,8 +3118,8 @@
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A95">
-        <v>55</v>
+      <c r="A95" t="s">
+        <v>144</v>
       </c>
       <c r="B95" t="s">
         <v>52</v>
@@ -3118,8 +3142,8 @@
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A96">
-        <v>55</v>
+      <c r="A96" t="s">
+        <v>144</v>
       </c>
       <c r="B96" t="s">
         <v>52</v>
@@ -3142,8 +3166,8 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A97">
-        <v>55</v>
+      <c r="A97" t="s">
+        <v>144</v>
       </c>
       <c r="B97" t="s">
         <v>52</v>
@@ -3166,8 +3190,8 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A98">
-        <v>55</v>
+      <c r="A98" t="s">
+        <v>144</v>
       </c>
       <c r="B98" t="s">
         <v>52</v>
@@ -3190,8 +3214,8 @@
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A99">
-        <v>55</v>
+      <c r="A99" t="s">
+        <v>144</v>
       </c>
       <c r="B99" t="s">
         <v>52</v>
@@ -3214,8 +3238,8 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A100">
-        <v>55</v>
+      <c r="A100" t="s">
+        <v>144</v>
       </c>
       <c r="B100" t="s">
         <v>52</v>
@@ -3238,8 +3262,8 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A101">
-        <v>55</v>
+      <c r="A101" t="s">
+        <v>144</v>
       </c>
       <c r="B101" t="s">
         <v>52</v>
@@ -3262,8 +3286,8 @@
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A102">
-        <v>55</v>
+      <c r="A102" t="s">
+        <v>144</v>
       </c>
       <c r="B102" t="s">
         <v>52</v>
@@ -3286,8 +3310,8 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A103">
-        <v>55</v>
+      <c r="A103" t="s">
+        <v>144</v>
       </c>
       <c r="B103" t="s">
         <v>52</v>
@@ -3310,8 +3334,8 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A104">
-        <v>55</v>
+      <c r="A104" t="s">
+        <v>144</v>
       </c>
       <c r="B104" t="s">
         <v>52</v>
@@ -3334,8 +3358,8 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A105">
-        <v>55</v>
+      <c r="A105" t="s">
+        <v>144</v>
       </c>
       <c r="B105" t="s">
         <v>52</v>
@@ -3358,8 +3382,8 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A106">
-        <v>55</v>
+      <c r="A106" t="s">
+        <v>144</v>
       </c>
       <c r="B106" t="s">
         <v>52</v>
@@ -3382,8 +3406,8 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A107">
-        <v>55</v>
+      <c r="A107" t="s">
+        <v>144</v>
       </c>
       <c r="B107" t="s">
         <v>52</v>
@@ -3406,8 +3430,8 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A108">
-        <v>55</v>
+      <c r="A108" t="s">
+        <v>144</v>
       </c>
       <c r="B108" t="s">
         <v>52</v>
@@ -3430,8 +3454,8 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A109">
-        <v>55</v>
+      <c r="A109" t="s">
+        <v>144</v>
       </c>
       <c r="B109" t="s">
         <v>52</v>
@@ -3453,8 +3477,8 @@
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A110">
-        <v>55</v>
+      <c r="A110" t="s">
+        <v>144</v>
       </c>
       <c r="B110" t="s">
         <v>52</v>
@@ -3477,8 +3501,8 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A111">
-        <v>55</v>
+      <c r="A111" t="s">
+        <v>144</v>
       </c>
       <c r="B111" t="s">
         <v>52</v>
@@ -3501,8 +3525,8 @@
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A112">
-        <v>55</v>
+      <c r="A112" t="s">
+        <v>144</v>
       </c>
       <c r="B112" t="s">
         <v>52</v>
@@ -3525,8 +3549,8 @@
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A113">
-        <v>55</v>
+      <c r="A113" t="s">
+        <v>144</v>
       </c>
       <c r="B113" t="s">
         <v>52</v>
@@ -3549,8 +3573,8 @@
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A114">
-        <v>55</v>
+      <c r="A114" t="s">
+        <v>144</v>
       </c>
       <c r="B114" t="s">
         <v>52</v>
@@ -3573,8 +3597,8 @@
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A115">
-        <v>55</v>
+      <c r="A115" t="s">
+        <v>144</v>
       </c>
       <c r="B115" t="s">
         <v>52</v>
@@ -3597,8 +3621,8 @@
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A116">
-        <v>55</v>
+      <c r="A116" t="s">
+        <v>144</v>
       </c>
       <c r="B116" t="s">
         <v>52</v>
@@ -3621,8 +3645,8 @@
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A117">
-        <v>55</v>
+      <c r="A117" t="s">
+        <v>144</v>
       </c>
       <c r="B117" t="s">
         <v>52</v>
@@ -3645,8 +3669,8 @@
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A118">
-        <v>55</v>
+      <c r="A118" t="s">
+        <v>144</v>
       </c>
       <c r="B118" t="s">
         <v>52</v>
@@ -3669,8 +3693,8 @@
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A119">
-        <v>55</v>
+      <c r="A119" t="s">
+        <v>144</v>
       </c>
       <c r="B119" t="s">
         <v>52</v>
@@ -3693,8 +3717,8 @@
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A120">
-        <v>55</v>
+      <c r="A120" t="s">
+        <v>144</v>
       </c>
       <c r="B120" t="s">
         <v>52</v>
@@ -3717,8 +3741,8 @@
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A121">
-        <v>55</v>
+      <c r="A121" t="s">
+        <v>144</v>
       </c>
       <c r="B121" t="s">
         <v>52</v>
@@ -3741,8 +3765,8 @@
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A122">
-        <v>55</v>
+      <c r="A122" t="s">
+        <v>144</v>
       </c>
       <c r="B122" t="s">
         <v>52</v>
@@ -3765,8 +3789,8 @@
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A123">
-        <v>55</v>
+      <c r="A123" t="s">
+        <v>144</v>
       </c>
       <c r="B123" t="s">
         <v>52</v>
@@ -3789,8 +3813,8 @@
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A124">
-        <v>55</v>
+      <c r="A124" t="s">
+        <v>144</v>
       </c>
       <c r="B124" t="s">
         <v>52</v>
@@ -3816,8 +3840,8 @@
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A125">
-        <v>55</v>
+      <c r="A125" t="s">
+        <v>144</v>
       </c>
       <c r="B125" t="s">
         <v>52</v>
@@ -3840,8 +3864,8 @@
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A126">
-        <v>55</v>
+      <c r="A126" t="s">
+        <v>144</v>
       </c>
       <c r="B126" t="s">
         <v>52</v>
@@ -3864,8 +3888,8 @@
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A127">
-        <v>56</v>
+      <c r="A127" t="s">
+        <v>145</v>
       </c>
       <c r="B127" t="s">
         <v>74</v>
@@ -3888,8 +3912,8 @@
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A128">
-        <v>56</v>
+      <c r="A128" t="s">
+        <v>145</v>
       </c>
       <c r="B128" t="s">
         <v>74</v>
@@ -3912,8 +3936,8 @@
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A129">
-        <v>56</v>
+      <c r="A129" t="s">
+        <v>145</v>
       </c>
       <c r="B129" t="s">
         <v>74</v>
@@ -3936,8 +3960,8 @@
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A130">
-        <v>56</v>
+      <c r="A130" t="s">
+        <v>145</v>
       </c>
       <c r="B130" t="s">
         <v>74</v>
@@ -3960,8 +3984,8 @@
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A131">
-        <v>56</v>
+      <c r="A131" t="s">
+        <v>145</v>
       </c>
       <c r="B131" t="s">
         <v>74</v>
@@ -3984,8 +4008,8 @@
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A132">
-        <v>56</v>
+      <c r="A132" t="s">
+        <v>145</v>
       </c>
       <c r="B132" t="s">
         <v>74</v>
@@ -4008,8 +4032,8 @@
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A133">
-        <v>56</v>
+      <c r="A133" t="s">
+        <v>145</v>
       </c>
       <c r="B133" t="s">
         <v>74</v>
@@ -4031,8 +4055,8 @@
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A134">
-        <v>56</v>
+      <c r="A134" t="s">
+        <v>145</v>
       </c>
       <c r="B134" t="s">
         <v>74</v>
@@ -4055,8 +4079,8 @@
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A135">
-        <v>56</v>
+      <c r="A135" t="s">
+        <v>145</v>
       </c>
       <c r="B135" t="s">
         <v>74</v>
@@ -4079,8 +4103,8 @@
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A136">
-        <v>56</v>
+      <c r="A136" t="s">
+        <v>145</v>
       </c>
       <c r="B136" t="s">
         <v>74</v>
@@ -4103,8 +4127,8 @@
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A137">
-        <v>56</v>
+      <c r="A137" t="s">
+        <v>145</v>
       </c>
       <c r="B137" t="s">
         <v>74</v>
@@ -4127,8 +4151,8 @@
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A138">
-        <v>56</v>
+      <c r="A138" t="s">
+        <v>145</v>
       </c>
       <c r="B138" t="s">
         <v>74</v>
@@ -4151,8 +4175,8 @@
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A139">
-        <v>56</v>
+      <c r="A139" t="s">
+        <v>145</v>
       </c>
       <c r="B139" t="s">
         <v>74</v>
@@ -4175,8 +4199,8 @@
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A140">
-        <v>56</v>
+      <c r="A140" t="s">
+        <v>145</v>
       </c>
       <c r="B140" t="s">
         <v>74</v>
@@ -4199,8 +4223,8 @@
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A141">
-        <v>56</v>
+      <c r="A141" t="s">
+        <v>145</v>
       </c>
       <c r="B141" t="s">
         <v>74</v>
@@ -4223,8 +4247,8 @@
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A142">
-        <v>56</v>
+      <c r="A142" t="s">
+        <v>145</v>
       </c>
       <c r="B142" t="s">
         <v>74</v>
@@ -4247,8 +4271,8 @@
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A143">
-        <v>56</v>
+      <c r="A143" t="s">
+        <v>145</v>
       </c>
       <c r="B143" t="s">
         <v>74</v>
@@ -4274,8 +4298,8 @@
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A144">
-        <v>56</v>
+      <c r="A144" t="s">
+        <v>145</v>
       </c>
       <c r="B144" t="s">
         <v>74</v>
@@ -4297,8 +4321,8 @@
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A145">
-        <v>56</v>
+      <c r="A145" t="s">
+        <v>145</v>
       </c>
       <c r="B145" t="s">
         <v>74</v>
@@ -4321,8 +4345,8 @@
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A146">
-        <v>56</v>
+      <c r="A146" t="s">
+        <v>145</v>
       </c>
       <c r="B146" t="s">
         <v>74</v>
@@ -4348,8 +4372,8 @@
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A147">
-        <v>56</v>
+      <c r="A147" t="s">
+        <v>145</v>
       </c>
       <c r="B147" t="s">
         <v>74</v>
@@ -4372,8 +4396,8 @@
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A148">
-        <v>56</v>
+      <c r="A148" t="s">
+        <v>145</v>
       </c>
       <c r="B148" t="s">
         <v>74</v>
@@ -4396,8 +4420,8 @@
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A149">
-        <v>56</v>
+      <c r="A149" t="s">
+        <v>145</v>
       </c>
       <c r="B149" t="s">
         <v>74</v>
@@ -4420,8 +4444,8 @@
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A150">
-        <v>56</v>
+      <c r="A150" t="s">
+        <v>145</v>
       </c>
       <c r="B150" t="s">
         <v>74</v>
@@ -4444,8 +4468,8 @@
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A151">
-        <v>56</v>
+      <c r="A151" t="s">
+        <v>145</v>
       </c>
       <c r="B151" t="s">
         <v>74</v>
@@ -4468,8 +4492,8 @@
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A152">
-        <v>56</v>
+      <c r="A152" t="s">
+        <v>145</v>
       </c>
       <c r="B152" t="s">
         <v>74</v>
@@ -4492,8 +4516,8 @@
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A153">
-        <v>57</v>
+      <c r="A153" t="s">
+        <v>146</v>
       </c>
       <c r="B153" t="s">
         <v>94</v>
@@ -4516,8 +4540,8 @@
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A154">
-        <v>57</v>
+      <c r="A154" t="s">
+        <v>146</v>
       </c>
       <c r="B154" t="s">
         <v>94</v>
@@ -4540,8 +4564,8 @@
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A155">
-        <v>57</v>
+      <c r="A155" t="s">
+        <v>146</v>
       </c>
       <c r="B155" t="s">
         <v>94</v>
@@ -4564,8 +4588,8 @@
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A156">
-        <v>57</v>
+      <c r="A156" t="s">
+        <v>146</v>
       </c>
       <c r="B156" t="s">
         <v>94</v>
@@ -4588,8 +4612,8 @@
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A157">
-        <v>57</v>
+      <c r="A157" t="s">
+        <v>146</v>
       </c>
       <c r="B157" t="s">
         <v>94</v>
@@ -4612,8 +4636,8 @@
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A158">
-        <v>57</v>
+      <c r="A158" t="s">
+        <v>146</v>
       </c>
       <c r="B158" t="s">
         <v>94</v>
@@ -4639,8 +4663,8 @@
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A159">
-        <v>57</v>
+      <c r="A159" t="s">
+        <v>146</v>
       </c>
       <c r="B159" t="s">
         <v>94</v>
@@ -4663,8 +4687,8 @@
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A160">
-        <v>57</v>
+      <c r="A160" t="s">
+        <v>146</v>
       </c>
       <c r="B160" t="s">
         <v>94</v>
@@ -4687,8 +4711,8 @@
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A161">
-        <v>57</v>
+      <c r="A161" t="s">
+        <v>146</v>
       </c>
       <c r="B161" t="s">
         <v>94</v>
@@ -4711,8 +4735,8 @@
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A162">
-        <v>57</v>
+      <c r="A162" t="s">
+        <v>146</v>
       </c>
       <c r="B162" t="s">
         <v>94</v>
@@ -4735,8 +4759,8 @@
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A163">
-        <v>57</v>
+      <c r="A163" t="s">
+        <v>146</v>
       </c>
       <c r="B163" t="s">
         <v>94</v>
@@ -4759,8 +4783,8 @@
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A164">
-        <v>57</v>
+      <c r="A164" t="s">
+        <v>146</v>
       </c>
       <c r="B164" t="s">
         <v>94</v>
@@ -4783,8 +4807,8 @@
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A165">
-        <v>57</v>
+      <c r="A165" t="s">
+        <v>146</v>
       </c>
       <c r="B165" t="s">
         <v>94</v>
@@ -4807,8 +4831,8 @@
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A166">
-        <v>57</v>
+      <c r="A166" t="s">
+        <v>146</v>
       </c>
       <c r="B166" t="s">
         <v>94</v>
@@ -4831,8 +4855,8 @@
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A167">
-        <v>57</v>
+      <c r="A167" t="s">
+        <v>146</v>
       </c>
       <c r="B167" t="s">
         <v>94</v>
@@ -4855,8 +4879,8 @@
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A168">
-        <v>57</v>
+      <c r="A168" t="s">
+        <v>146</v>
       </c>
       <c r="B168" t="s">
         <v>94</v>
@@ -4879,8 +4903,8 @@
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A169">
-        <v>57</v>
+      <c r="A169" t="s">
+        <v>146</v>
       </c>
       <c r="B169" t="s">
         <v>94</v>
@@ -4903,8 +4927,8 @@
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A170">
-        <v>57</v>
+      <c r="A170" t="s">
+        <v>146</v>
       </c>
       <c r="B170" t="s">
         <v>94</v>
@@ -4930,8 +4954,8 @@
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A171">
-        <v>57</v>
+      <c r="A171" t="s">
+        <v>146</v>
       </c>
       <c r="B171" t="s">
         <v>94</v>
@@ -4953,8 +4977,8 @@
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A172">
-        <v>57</v>
+      <c r="A172" t="s">
+        <v>146</v>
       </c>
       <c r="B172" t="s">
         <v>94</v>
@@ -4977,8 +5001,8 @@
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A173">
-        <v>57</v>
+      <c r="A173" t="s">
+        <v>146</v>
       </c>
       <c r="B173" t="s">
         <v>94</v>
@@ -5004,8 +5028,8 @@
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A174">
-        <v>57</v>
+      <c r="A174" t="s">
+        <v>146</v>
       </c>
       <c r="B174" t="s">
         <v>94</v>
@@ -5031,8 +5055,8 @@
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A175">
-        <v>57</v>
+      <c r="A175" t="s">
+        <v>146</v>
       </c>
       <c r="B175" t="s">
         <v>94</v>
@@ -5058,8 +5082,8 @@
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A176">
-        <v>57</v>
+      <c r="A176" t="s">
+        <v>146</v>
       </c>
       <c r="B176" t="s">
         <v>94</v>
@@ -5082,8 +5106,8 @@
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A177">
-        <v>57</v>
+      <c r="A177" t="s">
+        <v>146</v>
       </c>
       <c r="B177" t="s">
         <v>94</v>
@@ -5106,8 +5130,8 @@
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A178">
-        <v>57</v>
+      <c r="A178" t="s">
+        <v>146</v>
       </c>
       <c r="B178" t="s">
         <v>94</v>
@@ -5130,8 +5154,8 @@
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A179">
-        <v>57</v>
+      <c r="A179" t="s">
+        <v>146</v>
       </c>
       <c r="B179" t="s">
         <v>94</v>
@@ -5154,8 +5178,8 @@
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A180">
-        <v>57</v>
+      <c r="A180" t="s">
+        <v>146</v>
       </c>
       <c r="B180" t="s">
         <v>94</v>
@@ -5181,8 +5205,8 @@
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A181">
-        <v>57</v>
+      <c r="A181" t="s">
+        <v>146</v>
       </c>
       <c r="B181" t="s">
         <v>94</v>
@@ -5205,8 +5229,8 @@
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A182">
-        <v>57</v>
+      <c r="A182" t="s">
+        <v>146</v>
       </c>
       <c r="B182" t="s">
         <v>94</v>
@@ -5229,8 +5253,8 @@
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A183">
-        <v>57</v>
+      <c r="A183" t="s">
+        <v>146</v>
       </c>
       <c r="B183" t="s">
         <v>94</v>
@@ -5253,8 +5277,8 @@
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A184">
-        <v>57</v>
+      <c r="A184" t="s">
+        <v>146</v>
       </c>
       <c r="B184" t="s">
         <v>94</v>
@@ -5277,8 +5301,8 @@
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A185">
-        <v>57</v>
+      <c r="A185" t="s">
+        <v>146</v>
       </c>
       <c r="B185" t="s">
         <v>94</v>
@@ -5301,8 +5325,8 @@
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A186">
-        <v>57</v>
+      <c r="A186" t="s">
+        <v>146</v>
       </c>
       <c r="B186" t="s">
         <v>94</v>
@@ -5325,8 +5349,8 @@
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A187">
-        <v>57</v>
+      <c r="A187" t="s">
+        <v>146</v>
       </c>
       <c r="B187" t="s">
         <v>94</v>
@@ -5349,8 +5373,8 @@
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A188">
-        <v>76</v>
+      <c r="A188" t="s">
+        <v>147</v>
       </c>
       <c r="B188" t="s">
         <v>101</v>
@@ -5373,8 +5397,8 @@
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A189">
-        <v>76</v>
+      <c r="A189" t="s">
+        <v>147</v>
       </c>
       <c r="B189" t="s">
         <v>101</v>
@@ -5397,8 +5421,8 @@
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A190">
-        <v>76</v>
+      <c r="A190" t="s">
+        <v>147</v>
       </c>
       <c r="B190" t="s">
         <v>101</v>
@@ -5421,8 +5445,8 @@
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A191">
-        <v>76</v>
+      <c r="A191" t="s">
+        <v>147</v>
       </c>
       <c r="B191" t="s">
         <v>101</v>
@@ -5445,8 +5469,8 @@
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A192">
-        <v>76</v>
+      <c r="A192" t="s">
+        <v>147</v>
       </c>
       <c r="B192" t="s">
         <v>101</v>
@@ -5469,8 +5493,8 @@
       </c>
     </row>
     <row r="193" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A193">
-        <v>76</v>
+      <c r="A193" t="s">
+        <v>147</v>
       </c>
       <c r="B193" t="s">
         <v>101</v>
@@ -5493,8 +5517,8 @@
       </c>
     </row>
     <row r="194" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A194">
-        <v>76</v>
+      <c r="A194" t="s">
+        <v>147</v>
       </c>
       <c r="B194" t="s">
         <v>101</v>
@@ -5517,8 +5541,8 @@
       </c>
     </row>
     <row r="195" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A195">
-        <v>76</v>
+      <c r="A195" t="s">
+        <v>147</v>
       </c>
       <c r="B195" t="s">
         <v>101</v>
@@ -5541,8 +5565,8 @@
       </c>
     </row>
     <row r="196" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A196">
-        <v>76</v>
+      <c r="A196" t="s">
+        <v>147</v>
       </c>
       <c r="B196" t="s">
         <v>101</v>
@@ -5565,8 +5589,8 @@
       </c>
     </row>
     <row r="197" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A197">
-        <v>76</v>
+      <c r="A197" t="s">
+        <v>147</v>
       </c>
       <c r="B197" t="s">
         <v>101</v>
@@ -5589,8 +5613,8 @@
       </c>
     </row>
     <row r="198" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A198">
-        <v>76</v>
+      <c r="A198" t="s">
+        <v>147</v>
       </c>
       <c r="B198" t="s">
         <v>101</v>
@@ -5613,8 +5637,8 @@
       </c>
     </row>
     <row r="199" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A199">
-        <v>76</v>
+      <c r="A199" t="s">
+        <v>147</v>
       </c>
       <c r="B199" t="s">
         <v>101</v>
@@ -5637,8 +5661,8 @@
       </c>
     </row>
     <row r="200" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A200">
-        <v>76</v>
+      <c r="A200" t="s">
+        <v>147</v>
       </c>
       <c r="B200" t="s">
         <v>101</v>
@@ -5661,8 +5685,8 @@
       </c>
     </row>
     <row r="201" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A201">
-        <v>76</v>
+      <c r="A201" t="s">
+        <v>147</v>
       </c>
       <c r="B201" t="s">
         <v>101</v>
@@ -5685,8 +5709,8 @@
       </c>
     </row>
     <row r="202" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A202">
-        <v>76</v>
+      <c r="A202" t="s">
+        <v>147</v>
       </c>
       <c r="B202" t="s">
         <v>101</v>
@@ -5709,8 +5733,8 @@
       </c>
     </row>
     <row r="203" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A203">
-        <v>76</v>
+      <c r="A203" t="s">
+        <v>147</v>
       </c>
       <c r="B203" t="s">
         <v>101</v>
@@ -5733,8 +5757,8 @@
       </c>
     </row>
     <row r="204" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A204">
-        <v>76</v>
+      <c r="A204" t="s">
+        <v>147</v>
       </c>
       <c r="B204" t="s">
         <v>101</v>
@@ -5757,8 +5781,8 @@
       </c>
     </row>
     <row r="205" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A205">
-        <v>76</v>
+      <c r="A205" t="s">
+        <v>147</v>
       </c>
       <c r="B205" t="s">
         <v>101</v>
@@ -5781,8 +5805,8 @@
       </c>
     </row>
     <row r="206" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A206">
-        <v>76</v>
+      <c r="A206" t="s">
+        <v>147</v>
       </c>
       <c r="B206" t="s">
         <v>101</v>
@@ -5805,8 +5829,8 @@
       </c>
     </row>
     <row r="207" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A207">
-        <v>76</v>
+      <c r="A207" t="s">
+        <v>147</v>
       </c>
       <c r="B207" t="s">
         <v>101</v>
@@ -5829,8 +5853,8 @@
       </c>
     </row>
     <row r="208" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A208">
-        <v>76</v>
+      <c r="A208" t="s">
+        <v>147</v>
       </c>
       <c r="B208" t="s">
         <v>101</v>
@@ -5863,8 +5887,8 @@
       <c r="R208" s="2"/>
     </row>
     <row r="209" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A209">
-        <v>76</v>
+      <c r="A209" t="s">
+        <v>147</v>
       </c>
       <c r="B209" t="s">
         <v>101</v>
@@ -5897,8 +5921,8 @@
       <c r="R209" s="2"/>
     </row>
     <row r="210" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A210">
-        <v>76</v>
+      <c r="A210" t="s">
+        <v>147</v>
       </c>
       <c r="B210" t="s">
         <v>101</v>
@@ -5931,8 +5955,8 @@
       <c r="R210" s="2"/>
     </row>
     <row r="211" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A211">
-        <v>76</v>
+      <c r="A211" t="s">
+        <v>147</v>
       </c>
       <c r="B211" t="s">
         <v>101</v>
@@ -5965,8 +5989,8 @@
       <c r="R211" s="2"/>
     </row>
     <row r="212" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A212">
-        <v>76</v>
+      <c r="A212" t="s">
+        <v>147</v>
       </c>
       <c r="B212" t="s">
         <v>101</v>
@@ -5999,8 +6023,8 @@
       <c r="R212" s="2"/>
     </row>
     <row r="213" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A213">
-        <v>76</v>
+      <c r="A213" t="s">
+        <v>147</v>
       </c>
       <c r="B213" t="s">
         <v>101</v>
@@ -6033,8 +6057,8 @@
       <c r="R213" s="2"/>
     </row>
     <row r="214" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A214">
-        <v>78</v>
+      <c r="A214" t="s">
+        <v>148</v>
       </c>
       <c r="B214" t="s">
         <v>110</v>
@@ -6067,8 +6091,8 @@
       <c r="R214" s="2"/>
     </row>
     <row r="215" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A215">
-        <v>78</v>
+      <c r="A215" t="s">
+        <v>148</v>
       </c>
       <c r="B215" t="s">
         <v>110</v>
@@ -6101,8 +6125,8 @@
       <c r="R215" s="2"/>
     </row>
     <row r="216" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A216">
-        <v>78</v>
+      <c r="A216" t="s">
+        <v>148</v>
       </c>
       <c r="B216" t="s">
         <v>110</v>
@@ -6135,8 +6159,8 @@
       <c r="R216" s="2"/>
     </row>
     <row r="217" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A217">
-        <v>78</v>
+      <c r="A217" t="s">
+        <v>148</v>
       </c>
       <c r="B217" t="s">
         <v>110</v>
@@ -6169,8 +6193,8 @@
       <c r="R217" s="2"/>
     </row>
     <row r="218" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A218">
-        <v>78</v>
+      <c r="A218" t="s">
+        <v>148</v>
       </c>
       <c r="B218" t="s">
         <v>110</v>
@@ -6203,8 +6227,8 @@
       <c r="R218" s="2"/>
     </row>
     <row r="219" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A219">
-        <v>78</v>
+      <c r="A219" t="s">
+        <v>148</v>
       </c>
       <c r="B219" t="s">
         <v>110</v>
@@ -6237,8 +6261,8 @@
       <c r="R219" s="2"/>
     </row>
     <row r="220" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A220">
-        <v>78</v>
+      <c r="A220" t="s">
+        <v>148</v>
       </c>
       <c r="B220" t="s">
         <v>110</v>
@@ -6271,8 +6295,8 @@
       <c r="R220" s="2"/>
     </row>
     <row r="221" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A221">
-        <v>78</v>
+      <c r="A221" t="s">
+        <v>148</v>
       </c>
       <c r="B221" t="s">
         <v>110</v>
@@ -6305,8 +6329,8 @@
       <c r="R221" s="2"/>
     </row>
     <row r="222" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A222">
-        <v>78</v>
+      <c r="A222" t="s">
+        <v>148</v>
       </c>
       <c r="B222" t="s">
         <v>110</v>
@@ -6339,8 +6363,8 @@
       <c r="R222" s="2"/>
     </row>
     <row r="223" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A223">
-        <v>78</v>
+      <c r="A223" t="s">
+        <v>148</v>
       </c>
       <c r="B223" t="s">
         <v>110</v>
@@ -6373,8 +6397,8 @@
       <c r="R223" s="2"/>
     </row>
     <row r="224" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A224">
-        <v>78</v>
+      <c r="A224" t="s">
+        <v>148</v>
       </c>
       <c r="B224" t="s">
         <v>110</v>
@@ -6407,8 +6431,8 @@
       <c r="R224" s="2"/>
     </row>
     <row r="225" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A225">
-        <v>78</v>
+      <c r="A225" t="s">
+        <v>148</v>
       </c>
       <c r="B225" t="s">
         <v>110</v>
@@ -6441,8 +6465,8 @@
       <c r="R225" s="2"/>
     </row>
     <row r="226" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A226">
-        <v>78</v>
+      <c r="A226" t="s">
+        <v>148</v>
       </c>
       <c r="B226" t="s">
         <v>110</v>
@@ -6475,8 +6499,8 @@
       <c r="R226" s="2"/>
     </row>
     <row r="227" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A227">
-        <v>78</v>
+      <c r="A227" t="s">
+        <v>148</v>
       </c>
       <c r="B227" t="s">
         <v>110</v>
@@ -6509,8 +6533,8 @@
       <c r="R227" s="2"/>
     </row>
     <row r="228" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A228">
-        <v>78</v>
+      <c r="A228" t="s">
+        <v>148</v>
       </c>
       <c r="B228" t="s">
         <v>110</v>
@@ -6543,8 +6567,8 @@
       <c r="R228" s="2"/>
     </row>
     <row r="229" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A229">
-        <v>78</v>
+      <c r="A229" t="s">
+        <v>148</v>
       </c>
       <c r="B229" t="s">
         <v>110</v>
@@ -6577,8 +6601,8 @@
       <c r="R229" s="2"/>
     </row>
     <row r="230" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A230">
-        <v>78</v>
+      <c r="A230" t="s">
+        <v>148</v>
       </c>
       <c r="B230" t="s">
         <v>110</v>
@@ -6611,8 +6635,8 @@
       <c r="R230" s="2"/>
     </row>
     <row r="231" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A231">
-        <v>78</v>
+      <c r="A231" t="s">
+        <v>148</v>
       </c>
       <c r="B231" t="s">
         <v>110</v>
@@ -6645,8 +6669,8 @@
       <c r="R231" s="2"/>
     </row>
     <row r="232" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A232">
-        <v>78</v>
+      <c r="A232" t="s">
+        <v>148</v>
       </c>
       <c r="B232" t="s">
         <v>110</v>
@@ -6679,8 +6703,8 @@
       <c r="R232" s="2"/>
     </row>
     <row r="233" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A233">
-        <v>78</v>
+      <c r="A233" t="s">
+        <v>148</v>
       </c>
       <c r="B233" t="s">
         <v>110</v>
@@ -6713,8 +6737,8 @@
       <c r="R233" s="2"/>
     </row>
     <row r="234" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A234">
-        <v>78</v>
+      <c r="A234" t="s">
+        <v>148</v>
       </c>
       <c r="B234" t="s">
         <v>110</v>
@@ -6747,8 +6771,8 @@
       <c r="R234" s="2"/>
     </row>
     <row r="235" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A235">
-        <v>78</v>
+      <c r="A235" t="s">
+        <v>148</v>
       </c>
       <c r="B235" t="s">
         <v>110</v>
@@ -6781,8 +6805,8 @@
       <c r="R235" s="2"/>
     </row>
     <row r="236" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A236">
-        <v>78</v>
+      <c r="A236" t="s">
+        <v>148</v>
       </c>
       <c r="B236" t="s">
         <v>110</v>
@@ -6815,8 +6839,8 @@
       <c r="R236" s="2"/>
     </row>
     <row r="237" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A237">
-        <v>78</v>
+      <c r="A237" t="s">
+        <v>148</v>
       </c>
       <c r="B237" t="s">
         <v>110</v>
@@ -6849,8 +6873,8 @@
       <c r="R237" s="2"/>
     </row>
     <row r="238" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A238">
-        <v>78</v>
+      <c r="A238" t="s">
+        <v>148</v>
       </c>
       <c r="B238" t="s">
         <v>110</v>
@@ -6883,8 +6907,8 @@
       <c r="R238" s="2"/>
     </row>
     <row r="239" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A239">
-        <v>78</v>
+      <c r="A239" t="s">
+        <v>148</v>
       </c>
       <c r="B239" t="s">
         <v>110</v>
@@ -6917,8 +6941,8 @@
       <c r="R239" s="2"/>
     </row>
     <row r="240" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A240">
-        <v>78</v>
+      <c r="A240" t="s">
+        <v>148</v>
       </c>
       <c r="B240" t="s">
         <v>110</v>
@@ -6951,8 +6975,8 @@
       <c r="R240" s="2"/>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A241">
-        <v>78</v>
+      <c r="A241" t="s">
+        <v>148</v>
       </c>
       <c r="B241" t="s">
         <v>110</v>
@@ -6975,8 +6999,8 @@
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A242">
-        <v>78</v>
+      <c r="A242" t="s">
+        <v>148</v>
       </c>
       <c r="B242" t="s">
         <v>110</v>
@@ -6999,8 +7023,8 @@
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A243">
-        <v>78</v>
+      <c r="A243" t="s">
+        <v>148</v>
       </c>
       <c r="B243" t="s">
         <v>110</v>
@@ -7023,8 +7047,8 @@
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A244">
-        <v>78</v>
+      <c r="A244" t="s">
+        <v>148</v>
       </c>
       <c r="B244" t="s">
         <v>110</v>
@@ -7047,8 +7071,8 @@
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A245">
-        <v>78</v>
+      <c r="A245" t="s">
+        <v>148</v>
       </c>
       <c r="B245" t="s">
         <v>110</v>
@@ -7071,6 +7095,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I245" xr:uid="{83B3D47E-06F5-4A10-8434-91675729E215}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>